<commit_message>
Fix template sheet name
</commit_message>
<xml_diff>
--- a/eca-load-tests/src/main/resources/templates/load-test-report-template.xlsx
+++ b/eca-load-tests/src/main/resources/templates/load-test-report-template.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Отчет по классификаторам" sheetId="1" r:id="rId1"/>
+    <sheet name="Отчет по нагрузочному тестирова" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -369,11 +369,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -762,19 +762,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.6">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1143,7 +1143,7 @@
       <c r="G17" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="15" t="s">
         <v>43</v>
       </c>
       <c r="I17" s="11" t="s">

</xml_diff>

<commit_message>
add tps field in template
</commit_message>
<xml_diff>
--- a/eca-load-tests/src/main/resources/templates/load-test-report-template.xlsx
+++ b/eca-load-tests/src/main/resources/templates/load-test-report-template.xlsx
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A17" authorId="0">
+    <comment ref="A18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Классификатор</t>
   </si>
@@ -192,9 +192,6 @@
     <t>${evaluationTest.finished}</t>
   </si>
   <si>
-    <t>Стадия теста</t>
-  </si>
-  <si>
     <t>Настройки классификатора</t>
   </si>
   <si>
@@ -220,6 +217,15 @@
   </si>
   <si>
     <t>${evaluationTest.numAttributes}</t>
+  </si>
+  <si>
+    <t>Статус запроса</t>
+  </si>
+  <si>
+    <t>Кол-во запросов в сек.</t>
+  </si>
+  <si>
+    <t>${report.tps}</t>
   </si>
 </sst>
 </file>
@@ -343,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -372,8 +378,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -736,7 +744,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:K1"/>
@@ -762,19 +770,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.6">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1063,58 +1071,40 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="14.85" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" s="5" customFormat="1" ht="14.85" customHeight="1">
-      <c r="A16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>31</v>
-      </c>
+    <row r="15" spans="1:16" s="5" customFormat="1" ht="15.6">
+      <c r="A15" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" ht="14.85" customHeight="1">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1122,38 +1112,38 @@
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" s="5" customFormat="1" ht="14.85" customHeight="1">
-      <c r="A17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" s="11" t="s">
+      <c r="A17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>46</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1162,15 +1152,39 @@
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" s="5" customFormat="1" ht="14.85" customHeight="1">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
+      <c r="A18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1225,33 +1239,49 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16">
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
+    <row r="22" spans="1:16" s="5" customFormat="1" ht="14.85" customHeight="1">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
     </row>
     <row r="23" spans="1:16">
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-    </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1">
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="1:16" ht="15" customHeight="1">
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>